<commit_message>
xóa dòng cuối cùng thôi
</commit_message>
<xml_diff>
--- a/beautify_api/8.0.0/aspnet-core/src/BanHangBeautify.Web.Host/wwwroot/ImportExcelTemplate/KhachHang_ImportTemplate.xlsx
+++ b/beautify_api/8.0.0/aspnet-core/src/BanHangBeautify.Web.Host/wwwroot/ImportExcelTemplate/KhachHang_ImportTemplate.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Số điện  thoại</t>
   </si>
@@ -98,7 +98,10 @@
     </r>
   </si>
   <si>
-    <t>A Nam, bạn sếp</t>
+    <t>BS.Hoàng Văn Lợi</t>
+  </si>
+  <si>
+    <t>0978441444</t>
   </si>
 </sst>
 </file>
@@ -230,9 +233,6 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
@@ -250,6 +250,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -532,147 +535,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="40.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="30.85546875" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="29.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="40.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.85546875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>32402</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="6"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="3" t="s">
+      <c r="C4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>33116</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>1</v>
-      </c>
-      <c r="B7" s="3">
-        <v>2</v>
-      </c>
-      <c r="C7" s="3">
-        <v>3</v>
-      </c>
-      <c r="D7" s="3">
-        <v>4</v>
-      </c>
-      <c r="E7" s="3">
-        <v>5</v>
-      </c>
-      <c r="F7" s="3">
-        <v>6</v>
-      </c>
-      <c r="G7" s="3">
-        <v>7</v>
-      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Thông báo" error="Vui lòng chọn  đúng định dạng giới tính" sqref="E5:E1048576 E1 E3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Thông báo" error="Vui lòng chọn  đúng định dạng giới tính" sqref="E1 E3 E5:E1048576">
       <formula1>"Nữ, Nam,"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Thông báo" error="Vui lòng chọn  đúng định dạng giới tính" sqref="E4">

</xml_diff>

<commit_message>
importKhachHang: add coulmn {MaKhachHang}
</commit_message>
<xml_diff>
--- a/beautify_api/8.0.0/aspnet-core/src/BanHangBeautify.Web.Host/wwwroot/ImportExcelTemplate/KhachHang_ImportTemplate.xlsx
+++ b/beautify_api/8.0.0/aspnet-core/src/BanHangBeautify.Web.Host/wwwroot/ImportExcelTemplate/KhachHang_ImportTemplate.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Số điện  thoại</t>
   </si>
@@ -102,6 +102,15 @@
   </si>
   <si>
     <t>0978441444</t>
+  </si>
+  <si>
+    <t>Mã khách hàng</t>
+  </si>
+  <si>
+    <t>D012</t>
+  </si>
+  <si>
+    <t>KH05</t>
   </si>
 </sst>
 </file>
@@ -535,118 +544,129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="40.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="30.85546875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="2" width="29.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="40.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="30.85546875" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="10"/>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
     </row>
-    <row r="2" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4">
+      <c r="E3" s="4">
         <v>32402</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="5"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="4"/>
+      <c r="F4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="2"/>
       <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="4">
+      <c r="E5" s="4">
         <v>33116</v>
       </c>
-      <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Thông báo" error="Vui lòng chọn  đúng định dạng giới tính" sqref="E1 E3 E5:E1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Thông báo" error="Vui lòng chọn  đúng định dạng giới tính" sqref="F1 F3 F5:F1048576">
       <formula1>"Nữ, Nam,"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Thông báo" error="Vui lòng chọn  đúng định dạng giới tính" sqref="E4">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Thông báo" error="Vui lòng chọn  đúng định dạng giới tính" sqref="F4">
       <formula1>"Nữ, Nam,"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>